<commit_message>
CUpdated MLR Round 8 forecasts after correcting NY result
</commit_message>
<xml_diff>
--- a/seasons/RugbyUnion/MajorLeagueRugby/2023/forecasts/ReportRound8.xlsx
+++ b/seasons/RugbyUnion/MajorLeagueRugby/2023/forecasts/ReportRound8.xlsx
@@ -100,6 +100,24 @@
     <t>Houston, TX</t>
   </si>
   <si>
+    <t>TOR</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>Toronto, ON</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>CHI</t>
+  </si>
+  <si>
+    <t>Quincy, MA</t>
+  </si>
+  <si>
     <t>ATL</t>
   </si>
   <si>
@@ -116,24 +134,6 @@
   </si>
   <si>
     <t>Tukwila, WA</t>
-  </si>
-  <si>
-    <t>TOR</t>
-  </si>
-  <si>
-    <t>NY</t>
-  </si>
-  <si>
-    <t>Toronto, ON</t>
-  </si>
-  <si>
-    <t>NE</t>
-  </si>
-  <si>
-    <t>CHI</t>
-  </si>
-  <si>
-    <t>Quincy, MA</t>
   </si>
 </sst>
 </file>
@@ -181,6 +181,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFC81A2E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFC50A2A"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -198,14 +206,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFC81A2E"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -240,6 +240,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF0D408B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1F3250"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF031E41"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00653C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF00382D"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -259,30 +283,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0D408B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF1F3250"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF031E41"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00653C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -325,25 +325,25 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -743,19 +743,19 @@
       </c>
       <c r="C3" s="13"/>
       <c r="E3" s="13">
-        <v>0.4233693271666118</v>
+        <v>0.2898544077867403</v>
       </c>
       <c r="F3" s="13"/>
       <c r="H3" s="13">
-        <v>0.8962787833944006</v>
+        <v>0.4143042284928294</v>
       </c>
       <c r="I3" s="13"/>
       <c r="K3" s="13">
-        <v>0.2898544077867403</v>
+        <v>0.4233693271666118</v>
       </c>
       <c r="L3" s="13"/>
       <c r="N3" s="13">
-        <v>0.4143042284928294</v>
+        <v>0.8962787833944006</v>
       </c>
       <c r="O3" s="13"/>
     </row>
@@ -764,23 +764,23 @@
         <v>2</v>
       </c>
       <c r="B4" s="13">
-        <v>0.5609380148044518</v>
+        <v>0.5589249320120241</v>
       </c>
       <c r="C4" s="13"/>
       <c r="E4" s="13">
-        <v>0.977967604022646</v>
+        <v>0.1564147870618332</v>
       </c>
       <c r="F4" s="13"/>
       <c r="H4" s="13">
-        <v>0.8787914422125495</v>
+        <v>0.4050493048552056</v>
       </c>
       <c r="I4" s="13"/>
       <c r="K4" s="13">
-        <v>0.1581864017443524</v>
+        <v>0.9797872712205481</v>
       </c>
       <c r="L4" s="13"/>
       <c r="N4" s="13">
-        <v>0.4063617372215087</v>
+        <v>0.8809687625986774</v>
       </c>
       <c r="O4" s="13"/>
     </row>
@@ -789,23 +789,23 @@
         <v>3</v>
       </c>
       <c r="B5" s="12">
-        <v>35.96128033675343</v>
+        <v>35.83222323466912</v>
       </c>
       <c r="C5" s="12"/>
       <c r="E5" s="12">
-        <v>41.40414865058111</v>
+        <v>4.533751547289675</v>
       </c>
       <c r="F5" s="12"/>
       <c r="H5" s="12">
-        <v>78.76421246836745</v>
+        <v>16.78136397495928</v>
       </c>
       <c r="I5" s="12"/>
       <c r="K5" s="12">
-        <v>4.585102579752466</v>
+        <v>41.4811877783054</v>
       </c>
       <c r="L5" s="12"/>
       <c r="N5" s="12">
-        <v>16.8357386028563</v>
+        <v>78.95936107504131</v>
       </c>
       <c r="O5" s="12"/>
     </row>
@@ -814,34 +814,34 @@
         <v>4</v>
       </c>
       <c r="B6" s="14">
-        <v>0.8435998</v>
+        <v>0.84414</v>
       </c>
       <c r="C6" s="14">
-        <v>0.1274838</v>
+        <v>0.1267416</v>
       </c>
       <c r="E6" s="14">
-        <v>0.3968602</v>
+        <v>0.0226454</v>
       </c>
       <c r="F6" s="14">
-        <v>0.5644332</v>
+        <v>0.9743688</v>
       </c>
       <c r="H6" s="14">
-        <v>0.287433</v>
+        <v>0.9062972</v>
       </c>
       <c r="I6" s="14">
-        <v>0.6772144</v>
+        <v>0.0796834</v>
       </c>
       <c r="K6" s="14">
-        <v>0.0229702</v>
+        <v>0.4004586</v>
       </c>
       <c r="L6" s="14">
-        <v>0.9739878</v>
+        <v>0.561029</v>
       </c>
       <c r="N6" s="14">
-        <v>0.9058928000000001</v>
+        <v>0.2892026</v>
       </c>
       <c r="O6" s="14">
-        <v>0.0800496</v>
+        <v>0.6756529999999999</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -849,34 +849,34 @@
         <v>5</v>
       </c>
       <c r="B7" s="15">
-        <v>33.829978</v>
+        <v>33.8774584</v>
       </c>
       <c r="C7" s="15">
-        <v>22.5057156</v>
+        <v>22.5035152</v>
       </c>
       <c r="E7" s="15">
-        <v>26.114763</v>
+        <v>8.388645800000001</v>
       </c>
       <c r="F7" s="15">
-        <v>28.212484</v>
+        <v>28.980964</v>
       </c>
       <c r="H7" s="15">
-        <v>21.9001056</v>
+        <v>31.6785168</v>
       </c>
       <c r="I7" s="15">
-        <v>27.0994976</v>
+        <v>17.4978662</v>
       </c>
       <c r="K7" s="15">
-        <v>8.4295632</v>
+        <v>26.1238088</v>
       </c>
       <c r="L7" s="15">
-        <v>29.0853336</v>
+        <v>28.2389352</v>
       </c>
       <c r="N7" s="15">
-        <v>31.6829556</v>
+        <v>21.8799434</v>
       </c>
       <c r="O7" s="15">
-        <v>17.528049</v>
+        <v>27.082757</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -890,28 +890,28 @@
         <v>10</v>
       </c>
       <c r="E8" s="15">
+        <v>3</v>
+      </c>
+      <c r="F8" s="15">
+        <v>16</v>
+      </c>
+      <c r="H8" s="15">
+        <v>18</v>
+      </c>
+      <c r="I8" s="15">
+        <v>6</v>
+      </c>
+      <c r="K8" s="15">
         <v>15</v>
       </c>
-      <c r="F8" s="15">
+      <c r="L8" s="15">
         <v>15</v>
       </c>
-      <c r="H8" s="15">
+      <c r="N8" s="15">
         <v>10</v>
       </c>
-      <c r="I8" s="15">
-        <v>15</v>
-      </c>
-      <c r="K8" s="15">
-        <v>3</v>
-      </c>
-      <c r="L8" s="15">
-        <v>16</v>
-      </c>
-      <c r="N8" s="15">
-        <v>18</v>
-      </c>
       <c r="O8" s="15">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -925,28 +925,28 @@
         <v>13</v>
       </c>
       <c r="E9" s="15">
+        <v>3</v>
+      </c>
+      <c r="F9" s="15">
+        <v>19</v>
+      </c>
+      <c r="H9" s="15">
+        <v>21</v>
+      </c>
+      <c r="I9" s="15">
+        <v>9</v>
+      </c>
+      <c r="K9" s="15">
         <v>17</v>
       </c>
-      <c r="F9" s="15">
+      <c r="L9" s="15">
         <v>18</v>
       </c>
-      <c r="H9" s="15">
+      <c r="N9" s="15">
         <v>13</v>
       </c>
-      <c r="I9" s="15">
+      <c r="O9" s="15">
         <v>17</v>
-      </c>
-      <c r="K9" s="15">
-        <v>3</v>
-      </c>
-      <c r="L9" s="15">
-        <v>19</v>
-      </c>
-      <c r="N9" s="15">
-        <v>21</v>
-      </c>
-      <c r="O9" s="15">
-        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -960,28 +960,28 @@
         <v>14</v>
       </c>
       <c r="E10" s="15">
+        <v>3</v>
+      </c>
+      <c r="F10" s="15">
+        <v>21</v>
+      </c>
+      <c r="H10" s="15">
+        <v>23</v>
+      </c>
+      <c r="I10" s="15">
+        <v>11</v>
+      </c>
+      <c r="K10" s="15">
         <v>20</v>
       </c>
-      <c r="F10" s="15">
+      <c r="L10" s="15">
         <v>20</v>
       </c>
-      <c r="H10" s="15">
+      <c r="N10" s="15">
         <v>15</v>
       </c>
-      <c r="I10" s="15">
+      <c r="O10" s="15">
         <v>19</v>
-      </c>
-      <c r="K10" s="15">
-        <v>3</v>
-      </c>
-      <c r="L10" s="15">
-        <v>21</v>
-      </c>
-      <c r="N10" s="15">
-        <v>23</v>
-      </c>
-      <c r="O10" s="15">
-        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -989,34 +989,34 @@
         <v>9</v>
       </c>
       <c r="B11" s="15">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C11" s="15">
         <v>17</v>
       </c>
       <c r="E11" s="15">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="F11" s="15">
         <v>22</v>
       </c>
       <c r="H11" s="15">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="I11" s="15">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="K11" s="15">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="L11" s="15">
         <v>22</v>
       </c>
       <c r="N11" s="15">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="O11" s="15">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1030,28 +1030,28 @@
         <v>19</v>
       </c>
       <c r="E12" s="15">
+        <v>6</v>
+      </c>
+      <c r="F12" s="15">
+        <v>24</v>
+      </c>
+      <c r="H12" s="15">
+        <v>26</v>
+      </c>
+      <c r="I12" s="15">
+        <v>13</v>
+      </c>
+      <c r="K12" s="15">
         <v>22</v>
       </c>
-      <c r="F12" s="15">
+      <c r="L12" s="15">
         <v>23</v>
       </c>
-      <c r="H12" s="15">
+      <c r="N12" s="15">
         <v>17</v>
       </c>
-      <c r="I12" s="15">
+      <c r="O12" s="15">
         <v>22</v>
-      </c>
-      <c r="K12" s="15">
-        <v>6</v>
-      </c>
-      <c r="L12" s="15">
-        <v>24</v>
-      </c>
-      <c r="N12" s="15">
-        <v>26</v>
-      </c>
-      <c r="O12" s="15">
-        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1065,28 +1065,28 @@
         <v>19</v>
       </c>
       <c r="E13" s="15">
+        <v>6</v>
+      </c>
+      <c r="F13" s="15">
+        <v>25</v>
+      </c>
+      <c r="H13" s="15">
+        <v>27</v>
+      </c>
+      <c r="I13" s="15">
+        <v>14</v>
+      </c>
+      <c r="K13" s="15">
         <v>22</v>
       </c>
-      <c r="F13" s="15">
+      <c r="L13" s="15">
         <v>24</v>
       </c>
-      <c r="H13" s="15">
+      <c r="N13" s="15">
         <v>18</v>
       </c>
-      <c r="I13" s="15">
+      <c r="O13" s="15">
         <v>23</v>
-      </c>
-      <c r="K13" s="15">
-        <v>6</v>
-      </c>
-      <c r="L13" s="15">
-        <v>25</v>
-      </c>
-      <c r="N13" s="15">
-        <v>27</v>
-      </c>
-      <c r="O13" s="15">
-        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -1100,28 +1100,28 @@
         <v>19</v>
       </c>
       <c r="E14" s="15">
+        <v>6</v>
+      </c>
+      <c r="F14" s="15">
+        <v>26</v>
+      </c>
+      <c r="H14" s="15">
+        <v>29</v>
+      </c>
+      <c r="I14" s="15">
+        <v>15</v>
+      </c>
+      <c r="K14" s="15">
         <v>24</v>
       </c>
-      <c r="F14" s="15">
+      <c r="L14" s="15">
         <v>25</v>
       </c>
-      <c r="H14" s="15">
+      <c r="N14" s="15">
         <v>20</v>
       </c>
-      <c r="I14" s="15">
+      <c r="O14" s="15">
         <v>24</v>
-      </c>
-      <c r="K14" s="15">
-        <v>6</v>
-      </c>
-      <c r="L14" s="15">
-        <v>27</v>
-      </c>
-      <c r="N14" s="15">
-        <v>29</v>
-      </c>
-      <c r="O14" s="15">
-        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1135,28 +1135,28 @@
         <v>21</v>
       </c>
       <c r="E15" s="15">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="F15" s="15">
         <v>27</v>
       </c>
       <c r="H15" s="15">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="I15" s="15">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="K15" s="15">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="L15" s="15">
         <v>27</v>
       </c>
       <c r="N15" s="15">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="O15" s="15">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1170,28 +1170,28 @@
         <v>21</v>
       </c>
       <c r="E16" s="15">
+        <v>6</v>
+      </c>
+      <c r="F16" s="15">
+        <v>28</v>
+      </c>
+      <c r="H16" s="15">
+        <v>31</v>
+      </c>
+      <c r="I16" s="15">
+        <v>16</v>
+      </c>
+      <c r="K16" s="15">
         <v>26</v>
       </c>
-      <c r="F16" s="15">
+      <c r="L16" s="15">
         <v>27</v>
       </c>
-      <c r="H16" s="15">
+      <c r="N16" s="15">
         <v>21</v>
       </c>
-      <c r="I16" s="15">
+      <c r="O16" s="15">
         <v>27</v>
-      </c>
-      <c r="K16" s="15">
-        <v>6</v>
-      </c>
-      <c r="L16" s="15">
-        <v>28</v>
-      </c>
-      <c r="N16" s="15">
-        <v>31</v>
-      </c>
-      <c r="O16" s="15">
-        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1205,28 +1205,28 @@
         <v>22</v>
       </c>
       <c r="E17" s="15">
+        <v>8</v>
+      </c>
+      <c r="F17" s="15">
+        <v>29</v>
+      </c>
+      <c r="H17" s="15">
+        <v>32</v>
+      </c>
+      <c r="I17" s="15">
+        <v>17</v>
+      </c>
+      <c r="K17" s="15">
         <v>27</v>
       </c>
-      <c r="F17" s="15">
+      <c r="L17" s="15">
         <v>28</v>
       </c>
-      <c r="H17" s="15">
+      <c r="N17" s="15">
         <v>22</v>
       </c>
-      <c r="I17" s="15">
+      <c r="O17" s="15">
         <v>27</v>
-      </c>
-      <c r="K17" s="15">
-        <v>8</v>
-      </c>
-      <c r="L17" s="15">
-        <v>29</v>
-      </c>
-      <c r="N17" s="15">
-        <v>32</v>
-      </c>
-      <c r="O17" s="15">
-        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1240,28 +1240,28 @@
         <v>24</v>
       </c>
       <c r="E18" s="15">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="F18" s="15">
         <v>30</v>
       </c>
       <c r="H18" s="15">
+        <v>33</v>
+      </c>
+      <c r="I18" s="15">
+        <v>18</v>
+      </c>
+      <c r="K18" s="15">
+        <v>27</v>
+      </c>
+      <c r="L18" s="15">
+        <v>29</v>
+      </c>
+      <c r="N18" s="15">
         <v>23</v>
       </c>
-      <c r="I18" s="15">
+      <c r="O18" s="15">
         <v>29</v>
-      </c>
-      <c r="K18" s="15">
-        <v>9</v>
-      </c>
-      <c r="L18" s="15">
-        <v>30</v>
-      </c>
-      <c r="N18" s="15">
-        <v>33</v>
-      </c>
-      <c r="O18" s="15">
-        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -1275,28 +1275,28 @@
         <v>26</v>
       </c>
       <c r="E19" s="15">
+        <v>9</v>
+      </c>
+      <c r="F19" s="15">
+        <v>31</v>
+      </c>
+      <c r="H19" s="15">
+        <v>34</v>
+      </c>
+      <c r="I19" s="15">
+        <v>19</v>
+      </c>
+      <c r="K19" s="15">
         <v>29</v>
       </c>
-      <c r="F19" s="15">
+      <c r="L19" s="15">
         <v>30</v>
       </c>
-      <c r="H19" s="15">
+      <c r="N19" s="15">
         <v>24</v>
       </c>
-      <c r="I19" s="15">
+      <c r="O19" s="15">
         <v>29</v>
-      </c>
-      <c r="K19" s="15">
-        <v>9</v>
-      </c>
-      <c r="L19" s="15">
-        <v>32</v>
-      </c>
-      <c r="N19" s="15">
-        <v>34</v>
-      </c>
-      <c r="O19" s="15">
-        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -1310,28 +1310,28 @@
         <v>26</v>
       </c>
       <c r="E20" s="15">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="F20" s="15">
         <v>32</v>
       </c>
       <c r="H20" s="15">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="I20" s="15">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="K20" s="15">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="L20" s="15">
         <v>32</v>
       </c>
       <c r="N20" s="15">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="O20" s="15">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -1345,28 +1345,28 @@
         <v>26</v>
       </c>
       <c r="E21" s="15">
+        <v>9</v>
+      </c>
+      <c r="F21" s="15">
+        <v>33</v>
+      </c>
+      <c r="H21" s="15">
+        <v>36</v>
+      </c>
+      <c r="I21" s="15">
+        <v>21</v>
+      </c>
+      <c r="K21" s="15">
         <v>29</v>
       </c>
-      <c r="F21" s="15">
+      <c r="L21" s="15">
         <v>32</v>
       </c>
-      <c r="H21" s="15">
+      <c r="N21" s="15">
         <v>25</v>
       </c>
-      <c r="I21" s="15">
+      <c r="O21" s="15">
         <v>31</v>
-      </c>
-      <c r="K21" s="15">
-        <v>9</v>
-      </c>
-      <c r="L21" s="15">
-        <v>34</v>
-      </c>
-      <c r="N21" s="15">
-        <v>36</v>
-      </c>
-      <c r="O21" s="15">
-        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -1380,28 +1380,28 @@
         <v>28</v>
       </c>
       <c r="E22" s="15">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="F22" s="15">
         <v>34</v>
       </c>
       <c r="H22" s="15">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="I22" s="15">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K22" s="15">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="L22" s="15">
         <v>34</v>
       </c>
       <c r="N22" s="15">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="O22" s="15">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -1415,28 +1415,28 @@
         <v>28</v>
       </c>
       <c r="E23" s="15">
+        <v>12</v>
+      </c>
+      <c r="F23" s="15">
+        <v>36</v>
+      </c>
+      <c r="H23" s="15">
+        <v>39</v>
+      </c>
+      <c r="I23" s="15">
+        <v>23</v>
+      </c>
+      <c r="K23" s="15">
         <v>31</v>
       </c>
-      <c r="F23" s="15">
+      <c r="L23" s="15">
         <v>35</v>
       </c>
-      <c r="H23" s="15">
+      <c r="N23" s="15">
         <v>28</v>
       </c>
-      <c r="I23" s="15">
+      <c r="O23" s="15">
         <v>34</v>
-      </c>
-      <c r="K23" s="15">
-        <v>12</v>
-      </c>
-      <c r="L23" s="15">
-        <v>36</v>
-      </c>
-      <c r="N23" s="15">
-        <v>39</v>
-      </c>
-      <c r="O23" s="15">
-        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -1450,28 +1450,28 @@
         <v>31</v>
       </c>
       <c r="E24" s="15">
+        <v>12</v>
+      </c>
+      <c r="F24" s="15">
+        <v>37</v>
+      </c>
+      <c r="H24" s="15">
+        <v>40</v>
+      </c>
+      <c r="I24" s="15">
+        <v>24</v>
+      </c>
+      <c r="K24" s="15">
         <v>33</v>
-      </c>
-      <c r="F24" s="15">
-        <v>36</v>
-      </c>
-      <c r="H24" s="15">
-        <v>29</v>
-      </c>
-      <c r="I24" s="15">
-        <v>35</v>
-      </c>
-      <c r="K24" s="15">
-        <v>12</v>
       </c>
       <c r="L24" s="15">
         <v>37</v>
       </c>
       <c r="N24" s="15">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="O24" s="15">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -1485,28 +1485,28 @@
         <v>33</v>
       </c>
       <c r="E25" s="15">
+        <v>13</v>
+      </c>
+      <c r="F25" s="15">
+        <v>39</v>
+      </c>
+      <c r="H25" s="15">
+        <v>42</v>
+      </c>
+      <c r="I25" s="15">
+        <v>26</v>
+      </c>
+      <c r="K25" s="15">
         <v>34</v>
-      </c>
-      <c r="F25" s="15">
-        <v>38</v>
-      </c>
-      <c r="H25" s="15">
-        <v>30</v>
-      </c>
-      <c r="I25" s="15">
-        <v>37</v>
-      </c>
-      <c r="K25" s="15">
-        <v>14</v>
       </c>
       <c r="L25" s="15">
         <v>39</v>
       </c>
       <c r="N25" s="15">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="O25" s="15">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:15">
@@ -1520,28 +1520,28 @@
         <v>35</v>
       </c>
       <c r="E26" s="15">
+        <v>17</v>
+      </c>
+      <c r="F26" s="15">
+        <v>41</v>
+      </c>
+      <c r="H26" s="15">
+        <v>45</v>
+      </c>
+      <c r="I26" s="15">
+        <v>28</v>
+      </c>
+      <c r="K26" s="15">
         <v>36</v>
-      </c>
-      <c r="F26" s="15">
-        <v>40</v>
-      </c>
-      <c r="H26" s="15">
-        <v>33</v>
-      </c>
-      <c r="I26" s="15">
-        <v>39</v>
-      </c>
-      <c r="K26" s="15">
-        <v>18</v>
       </c>
       <c r="L26" s="15">
         <v>41</v>
       </c>
       <c r="N26" s="15">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="O26" s="15">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>